<commit_message>
final commit with list of project requirements
</commit_message>
<xml_diff>
--- a/project requirements.xlsx
+++ b/project requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>Functional Requirements</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Compose Tweet</t>
-  </si>
-  <si>
-    <t>Stretch</t>
   </si>
   <si>
     <t>When a user clicks a tweet's "Like" button, the "Like" count is updated</t>
@@ -253,13 +250,16 @@
       </rPr>
       <t> is cleared, and the Character Counter is reset (to 140)</t>
     </r>
+  </si>
+  <si>
+    <t>Stretch - only if time.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,8 +290,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +308,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -329,6 +342,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -681,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15">
@@ -689,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15">
@@ -697,7 +711,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15">
@@ -715,7 +729,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15">
@@ -723,7 +737,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15">
@@ -731,7 +745,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15">
@@ -744,7 +758,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15">
@@ -752,15 +766,15 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15">
@@ -768,7 +782,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15">
@@ -776,7 +790,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15">
@@ -789,7 +803,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15">
@@ -807,7 +821,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15">
@@ -815,7 +829,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15">
@@ -823,7 +837,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15">
@@ -831,7 +845,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15">
@@ -844,7 +858,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15">
@@ -852,7 +866,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15">
@@ -872,10 +886,10 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15">
@@ -883,7 +897,7 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15">
@@ -891,7 +905,7 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15">
@@ -901,18 +915,18 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15">
@@ -922,33 +936,40 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15">
+      <c r="A39" s="3"/>
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" spans="1:2" ht="15">
+      <c r="A40" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15">
-      <c r="A39" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15">
-      <c r="A40" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B40" s="1"/>
     </row>
     <row r="41" spans="1:2" ht="15">
       <c r="A41" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" ht="15">
+      <c r="A42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
git push with final requirments - list didnt update last commit
</commit_message>
<xml_diff>
--- a/project requirements.xlsx
+++ b/project requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -676,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>

</xml_diff>